<commit_message>
last two miners assignment 2
</commit_message>
<xml_diff>
--- a/assignment2/excel.xlsx
+++ b/assignment2/excel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
   <si>
     <t>Noise percentage</t>
   </si>
@@ -23,7 +23,7 @@
     <t>Fitness</t>
   </si>
   <si>
-    <t>Remove Head</t>
+    <t>Add Event</t>
   </si>
 </sst>
 </file>
@@ -189,39 +189,6 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n" s="2">
-        <v>80.0</v>
-      </c>
-      <c r="B10" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="C10" t="n" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n" s="2">
-        <v>90.0</v>
-      </c>
-      <c r="B11" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="C11" t="n" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n" s="2">
-        <v>100.0</v>
-      </c>
-      <c r="B12" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="C12" t="n" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
wat een kut zooi
</commit_message>
<xml_diff>
--- a/assignment2/excel.xlsx
+++ b/assignment2/excel.xlsx
@@ -119,9 +119,7 @@
       <c r="B3" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="C3" t="n" s="2">
-        <v>1.0</v>
-      </c>
+      <c r="C3"/>
     </row>
     <row r="4">
       <c r="A4" t="n" s="2">
@@ -130,9 +128,7 @@
       <c r="B4" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="C4" t="n" s="2">
-        <v>1.0</v>
-      </c>
+      <c r="C4"/>
     </row>
     <row r="5">
       <c r="A5" t="n" s="2">
@@ -141,9 +137,7 @@
       <c r="B5" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="C5" t="n" s="2">
-        <v>1.0</v>
-      </c>
+      <c r="C5"/>
     </row>
     <row r="6">
       <c r="A6" t="n" s="2">
@@ -152,9 +146,7 @@
       <c r="B6" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="C6" t="n" s="2">
-        <v>1.0</v>
-      </c>
+      <c r="C6"/>
     </row>
     <row r="7">
       <c r="A7" t="n" s="2">
@@ -163,9 +155,7 @@
       <c r="B7" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="C7" t="n" s="2">
-        <v>1.0</v>
-      </c>
+      <c r="C7"/>
     </row>
     <row r="8">
       <c r="A8" t="n" s="2">
@@ -174,9 +164,7 @@
       <c r="B8" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="C8" t="n" s="2">
-        <v>1.0</v>
-      </c>
+      <c r="C8"/>
     </row>
     <row r="9">
       <c r="A9" t="n" s="2">
@@ -185,9 +173,7 @@
       <c r="B9" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="C9" t="n" s="2">
-        <v>1.0</v>
-      </c>
+      <c r="C9"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>